<commit_message>
Atualizando documentação - diagrama de classses
</commit_message>
<xml_diff>
--- a/docs/Dicionário de Dados.xlsx
+++ b/docs/Dicionário de Dados.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="177">
   <si>
     <t xml:space="preserve">OTIMIZADOR DE BANCO DE DADOS</t>
   </si>
@@ -174,6 +174,18 @@
     <t xml:space="preserve">Nome da base</t>
   </si>
   <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ativo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Entidade:  Database_Configurations</t>
   </si>
   <si>
@@ -181,15 +193,6 @@
   </si>
   <si>
     <t xml:space="preserve">Identificador Único do Banco de dados</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ativo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bit</t>
   </si>
   <si>
     <t xml:space="preserve">Se o banco está ativo ou não</t>
@@ -758,7 +761,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -874,21 +877,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1015"/>
+  <dimension ref="A1:H1016"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="9" style="0" width="7.62"/>
   </cols>
@@ -961,7 +963,7 @@
       <c r="G6" s="6"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1"/>
       <c r="B7" s="7" t="s">
         <v>4</v>
@@ -983,7 +985,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="B8" s="9" t="s">
         <v>10</v>
@@ -1137,7 +1139,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="9" t="s">
         <v>10</v>
@@ -1159,7 +1161,7 @@
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1"/>
       <c r="B19" s="9" t="s">
         <v>15</v>
@@ -1181,7 +1183,7 @@
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="9" t="s">
         <v>19</v>
@@ -1229,7 +1231,7 @@
       <c r="G22" s="6"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1"/>
       <c r="B23" s="7" t="s">
         <v>24</v>
@@ -1265,7 +1267,7 @@
       <c r="G24" s="11"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
       <c r="B25" s="9" t="s">
         <v>15</v>
@@ -1339,7 +1341,7 @@
       </c>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1"/>
       <c r="B30" s="9" t="s">
         <v>10</v>
@@ -1377,7 +1379,7 @@
       </c>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1"/>
       <c r="B32" s="9" t="s">
         <v>19</v>
@@ -1531,7 +1533,7 @@
       </c>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
       <c r="B42" s="9" t="s">
         <v>15</v>
@@ -1589,361 +1591,361 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1"/>
-      <c r="B45" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
+      <c r="B45" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="H45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1"/>
-      <c r="B46" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G46" s="8"/>
+      <c r="B46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
       <c r="H46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1"/>
-      <c r="B47" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="G47" s="11"/>
+      <c r="B47" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="8"/>
       <c r="H47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1"/>
+      <c r="B48" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="11"/>
       <c r="H48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1"/>
-      <c r="B49" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
       <c r="H49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1"/>
-      <c r="B50" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
+      <c r="B50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
       <c r="H50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1"/>
-      <c r="B51" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E51" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B51" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
       <c r="H51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1"/>
-      <c r="B52" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>32</v>
+      <c r="B52" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1"/>
       <c r="B53" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G53" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1"/>
       <c r="B54" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="9"/>
       <c r="G54" s="11" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1"/>
       <c r="B55" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
       <c r="G55" s="11" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="H55" s="1"/>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1"/>
       <c r="B56" s="9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G56" s="11" t="s">
         <v>56</v>
       </c>
       <c r="H56" s="1"/>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1"/>
-      <c r="B57" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
+      <c r="B57" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="H57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1"/>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1"/>
+      <c r="B59" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C59" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="7"/>
-      <c r="E58" s="8" t="s">
+      <c r="D59" s="7"/>
+      <c r="E59" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F59" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G58" s="8"/>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="1"/>
-      <c r="B59" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F59" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G59" s="11"/>
+      <c r="G59" s="8"/>
       <c r="H59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1"/>
       <c r="B60" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="D60" s="10"/>
-      <c r="E60" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F60" s="10" t="s">
-        <v>31</v>
+      <c r="E60" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="G60" s="11"/>
       <c r="H60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1"/>
+      <c r="B61" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G61" s="11"/>
       <c r="H61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1"/>
-      <c r="B62" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
       <c r="H62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1"/>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
       <c r="H63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1"/>
-      <c r="B64" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B64" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
       <c r="H64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1"/>
-      <c r="B65" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="9"/>
-      <c r="G65" s="11" t="s">
-        <v>61</v>
+      <c r="B65" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="H65" s="1"/>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1"/>
       <c r="B66" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E66" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="F66" s="9"/>
       <c r="G66" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1"/>
       <c r="B67" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D67" s="11" t="s">
         <v>17</v>
@@ -1951,217 +1953,215 @@
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1"/>
       <c r="B68" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E68" s="9"/>
-      <c r="F68" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="F68" s="9"/>
       <c r="G68" s="11" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="H68" s="1"/>
     </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1"/>
       <c r="B69" s="9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C69" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1"/>
+      <c r="B70" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="D70" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="11" t="s">
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H69" s="1"/>
-    </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1"/>
-      <c r="B70" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6"/>
       <c r="H70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1"/>
-      <c r="B71" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D71" s="7"/>
-      <c r="E71" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G71" s="8"/>
+      <c r="B71" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
       <c r="H71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1"/>
-      <c r="B72" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F72" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="G72" s="11"/>
+      <c r="B72" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G72" s="8"/>
       <c r="H72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1"/>
+      <c r="B73" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G73" s="11"/>
       <c r="H73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1"/>
-      <c r="B74" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
       <c r="H74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1"/>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
-      <c r="F75" s="6"/>
-      <c r="G75" s="6"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5"/>
+      <c r="G75" s="5"/>
       <c r="H75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1"/>
-      <c r="B76" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B76" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
       <c r="H76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1"/>
-      <c r="B77" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C77" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F77" s="9"/>
-      <c r="G77" s="11" t="s">
-        <v>69</v>
+      <c r="B77" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="H77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E78" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="F78" s="9"/>
       <c r="G78" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1"/>
       <c r="B79" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C79" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1"/>
       <c r="B80" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="E80" s="9"/>
-      <c r="F80" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="F80" s="9"/>
       <c r="G80" s="11" t="s">
         <v>75</v>
       </c>
@@ -2170,38 +2170,38 @@
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1"/>
       <c r="B81" s="9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E81" s="9"/>
-      <c r="F81" s="9"/>
+      <c r="F81" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G81" s="11" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="H81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1"/>
       <c r="B82" s="9" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C82" s="10" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="E82" s="9"/>
-      <c r="F82" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="F82" s="9"/>
       <c r="G82" s="11" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="H82" s="1"/>
     </row>
@@ -2211,262 +2211,264 @@
         <v>77</v>
       </c>
       <c r="C83" s="10" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="E83" s="9"/>
-      <c r="F83" s="9"/>
+      <c r="F83" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G83" s="11" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="H83" s="1"/>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1"/>
       <c r="B84" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
       <c r="G84" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H84" s="1"/>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1"/>
-      <c r="B85" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
+      <c r="B85" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="H85" s="1"/>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="1"/>
-      <c r="B86" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D86" s="7"/>
-      <c r="E86" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G86" s="8"/>
+      <c r="B86" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
       <c r="H86" s="1"/>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="1"/>
-      <c r="B87" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D87" s="10"/>
-      <c r="E87" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G87" s="11"/>
+      <c r="B87" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G87" s="8"/>
       <c r="H87" s="1"/>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="1"/>
       <c r="B88" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D88" s="10"/>
-      <c r="E88" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F88" s="10" t="s">
-        <v>60</v>
+      <c r="E88" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F88" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="1"/>
-      <c r="G89" s="13"/>
+      <c r="B89" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F89" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G89" s="11"/>
       <c r="H89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="1"/>
-      <c r="B90" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
+      <c r="G90" s="13"/>
       <c r="H90" s="1"/>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="1"/>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
-      <c r="F91" s="6"/>
-      <c r="G91" s="6"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="5"/>
       <c r="H91" s="1"/>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="1"/>
-      <c r="B92" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B92" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
       <c r="H92" s="1"/>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1"/>
-      <c r="B93" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E93" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F93" s="9"/>
-      <c r="G93" s="11" t="s">
-        <v>88</v>
+      <c r="B93" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F93" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G93" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="H93" s="1"/>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="1"/>
-      <c r="B94" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>89</v>
+      <c r="B94" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="D94" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E94" s="14"/>
+      <c r="E94" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="F94" s="9"/>
-      <c r="G94" s="16" t="s">
-        <v>90</v>
+      <c r="G94" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="H94" s="1"/>
     </row>
-    <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1"/>
       <c r="B95" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C95" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E95" s="14"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="16" t="s">
         <v>91</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E95" s="9"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="H95" s="1"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="1"/>
       <c r="B96" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>92</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E96" s="9"/>
-      <c r="F96" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="F96" s="9"/>
       <c r="G96" s="11" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="H96" s="1"/>
     </row>
-    <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1"/>
       <c r="B97" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>93</v>
+        <v>35</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="E97" s="9"/>
-      <c r="F97" s="9"/>
+      <c r="F97" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G97" s="11" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="H97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="1"/>
       <c r="B98" s="14" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D98" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
       <c r="G98" s="11" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="H98" s="1"/>
     </row>
@@ -2476,273 +2478,271 @@
         <v>77</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
       <c r="G99" s="11" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="H99" s="1"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="1"/>
       <c r="B100" s="14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C100" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H100" s="1"/>
+    </row>
+    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1"/>
+      <c r="B101" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C101" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D100" s="11" t="s">
+      <c r="D101" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E100" s="9"/>
-      <c r="F100" s="9" t="s">
+      <c r="E101" s="9"/>
+      <c r="F101" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G100" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="H100" s="1"/>
-    </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1"/>
-      <c r="B101" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
+      <c r="G101" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="H101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="1"/>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="1"/>
+    </row>
+    <row r="103" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1"/>
+      <c r="B103" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C102" s="7" t="s">
+      <c r="C103" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D102" s="7"/>
-      <c r="E102" s="8" t="s">
+      <c r="D103" s="7"/>
+      <c r="E103" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F102" s="8" t="s">
+      <c r="F103" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G102" s="8"/>
-      <c r="H102" s="1"/>
-    </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1"/>
-      <c r="B103" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D103" s="10"/>
-      <c r="E103" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F103" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G103" s="11"/>
+      <c r="G103" s="8"/>
       <c r="H103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="1"/>
       <c r="B104" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D104" s="10"/>
-      <c r="E104" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F104" s="16" t="s">
-        <v>60</v>
+      <c r="E104" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F104" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="G104" s="11"/>
       <c r="H104" s="1"/>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
+      <c r="B105" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D105" s="10"/>
+      <c r="E105" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F105" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G105" s="11"/>
       <c r="H105" s="1"/>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
-      <c r="B106" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="5"/>
-      <c r="G106" s="5"/>
       <c r="H106" s="1"/>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="1"/>
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-      <c r="E107" s="6"/>
-      <c r="F107" s="6"/>
-      <c r="G107" s="6"/>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+      <c r="F107" s="5"/>
+      <c r="G107" s="5"/>
       <c r="H107" s="1"/>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="1"/>
-      <c r="B108" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C108" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F108" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G108" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B108" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
       <c r="H108" s="1"/>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="1"/>
-      <c r="B109" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C109" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D109" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F109" s="9"/>
-      <c r="G109" s="18" t="s">
-        <v>101</v>
+      <c r="B109" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D109" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G109" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="H109" s="1"/>
     </row>
-    <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="1"/>
       <c r="B110" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C110" s="18" t="s">
-        <v>102</v>
+        <v>10</v>
+      </c>
+      <c r="C110" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="D110" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E110" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="F110" s="9"/>
       <c r="G110" s="18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H110" s="1"/>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="1"/>
       <c r="B111" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C111" s="18" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="E111" s="9"/>
       <c r="F111" s="9"/>
       <c r="G111" s="18" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="H111" s="1"/>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="1"/>
       <c r="B112" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C112" s="18" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="D112" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
       <c r="G112" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="H112" s="1"/>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="1"/>
       <c r="B113" s="9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D113" s="11" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E113" s="9"/>
       <c r="F113" s="9"/>
       <c r="G113" s="18" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="H113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="1"/>
       <c r="B114" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C114" s="17" t="s">
-        <v>105</v>
+        <v>50</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>97</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="E114" s="9"/>
-      <c r="F114" s="14" t="s">
-        <v>13</v>
-      </c>
+      <c r="F114" s="9"/>
       <c r="G114" s="18" t="s">
-        <v>106</v>
+        <v>6</v>
       </c>
       <c r="H114" s="1"/>
     </row>
-    <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="1"/>
       <c r="B115" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C115" s="18" t="s">
-        <v>107</v>
+      <c r="C115" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="D115" s="11" t="s">
         <v>12</v>
@@ -2752,236 +2752,238 @@
         <v>13</v>
       </c>
       <c r="G115" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H115" s="1"/>
     </row>
-    <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="1"/>
       <c r="B116" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C116" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116" s="9"/>
+      <c r="F116" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" s="18" t="s">
         <v>109</v>
-      </c>
-      <c r="D116" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E116" s="9"/>
-      <c r="F116" s="9"/>
-      <c r="G116" s="18" t="s">
-        <v>110</v>
       </c>
       <c r="H116" s="1"/>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="1"/>
       <c r="B117" s="9" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="C117" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="E117" s="9"/>
       <c r="F117" s="9"/>
       <c r="G117" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="H117" s="1"/>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="1"/>
       <c r="B118" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C118" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D118" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E118" s="9"/>
       <c r="F118" s="9"/>
       <c r="G118" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H118" s="1"/>
     </row>
-    <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1"/>
       <c r="B119" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C119" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D119" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E119" s="9"/>
       <c r="F119" s="9"/>
       <c r="G119" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="B120" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C120" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="E120" s="9"/>
       <c r="F120" s="9"/>
       <c r="G120" s="18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H120" s="1"/>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
       <c r="B121" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C121" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D121" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E121" s="9"/>
       <c r="F121" s="9"/>
       <c r="G121" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H121" s="1"/>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
       <c r="B122" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C122" s="18" t="s">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="D122" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E122" s="9"/>
       <c r="F122" s="9"/>
       <c r="G122" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H122" s="1"/>
     </row>
-    <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="B123" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="C123" s="18" t="s">
+      <c r="H123" s="1"/>
+    </row>
+    <row r="124" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1"/>
+      <c r="B124" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C124" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="D123" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E123" s="9"/>
-      <c r="F123" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G123" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="H123" s="1"/>
-    </row>
-    <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1"/>
-      <c r="B124" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="C124" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="D124" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E124" s="9"/>
-      <c r="F124" s="9"/>
+      <c r="F124" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="G124" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H124" s="1"/>
+    </row>
+    <row r="125" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="1"/>
+      <c r="B125" s="9" t="n">
+        <v>16</v>
+      </c>
+      <c r="C125" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="H124" s="1"/>
-    </row>
-    <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1"/>
-      <c r="B125" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
-      <c r="E125" s="6"/>
-      <c r="F125" s="6"/>
-      <c r="G125" s="6"/>
+      <c r="D125" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="17" t="s">
+        <v>91</v>
+      </c>
       <c r="H125" s="1"/>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="1"/>
-      <c r="B126" s="7" t="s">
+      <c r="B126" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="1"/>
+    </row>
+    <row r="127" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1"/>
+      <c r="B127" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C126" s="7" t="s">
+      <c r="C127" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D126" s="7"/>
-      <c r="E126" s="8" t="s">
+      <c r="D127" s="7"/>
+      <c r="E127" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F126" s="8" t="s">
+      <c r="F127" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G126" s="8"/>
-      <c r="H126" s="1"/>
-    </row>
-    <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1"/>
-      <c r="B127" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C127" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D127" s="10"/>
-      <c r="E127" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F127" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G127" s="11"/>
+      <c r="G127" s="8"/>
       <c r="H127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="1"/>
-      <c r="B128" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C128" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D128" s="15"/>
-      <c r="E128" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F128" s="16" t="s">
-        <v>87</v>
+      <c r="B128" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C128" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D128" s="10"/>
+      <c r="E128" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F128" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="G128" s="11"/>
       <c r="H128" s="1"/>
@@ -2989,178 +2991,178 @@
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="1"/>
       <c r="B129" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D129" s="15"/>
-      <c r="E129" s="18" t="s">
-        <v>107</v>
+      <c r="E129" s="17" t="s">
+        <v>106</v>
       </c>
       <c r="F129" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G129" s="11"/>
       <c r="H129" s="1"/>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="1"/>
+      <c r="B130" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C130" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="D130" s="15"/>
+      <c r="E130" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G130" s="11"/>
       <c r="H130" s="1"/>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="1"/>
-      <c r="B131" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C131" s="5"/>
-      <c r="D131" s="5"/>
-      <c r="E131" s="5"/>
-      <c r="F131" s="5"/>
-      <c r="G131" s="5"/>
       <c r="H131" s="1"/>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="1"/>
-      <c r="B132" s="6" t="s">
+      <c r="B132" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C132" s="6"/>
-      <c r="D132" s="6"/>
-      <c r="E132" s="6"/>
-      <c r="F132" s="6"/>
-      <c r="G132" s="6"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
       <c r="H132" s="1"/>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="1"/>
-      <c r="B133" s="7" t="s">
+      <c r="B133" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C133" s="6"/>
+      <c r="D133" s="6"/>
+      <c r="E133" s="6"/>
+      <c r="F133" s="6"/>
+      <c r="G133" s="6"/>
+      <c r="H133" s="1"/>
+    </row>
+    <row r="134" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1"/>
+      <c r="B134" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C133" s="7" t="s">
+      <c r="C134" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D133" s="8" t="s">
+      <c r="D134" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E133" s="8" t="s">
+      <c r="E134" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F133" s="8" t="s">
+      <c r="F134" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G133" s="8" t="s">
+      <c r="G134" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H133" s="1"/>
-    </row>
-    <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1"/>
-      <c r="B134" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C134" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D134" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E134" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F134" s="9"/>
-      <c r="G134" s="18" t="s">
-        <v>134</v>
-      </c>
       <c r="H134" s="1"/>
     </row>
-    <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1"/>
       <c r="B135" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C135" s="18" t="s">
-        <v>135</v>
+        <v>10</v>
+      </c>
+      <c r="C135" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E135" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="E135" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="F135" s="9"/>
       <c r="G135" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H135" s="1"/>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="1"/>
       <c r="B136" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C136" s="18" t="s">
-        <v>20</v>
+        <v>136</v>
       </c>
       <c r="D136" s="11" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="E136" s="9"/>
       <c r="F136" s="9"/>
       <c r="G136" s="18" t="s">
-        <v>22</v>
+        <v>137</v>
       </c>
       <c r="H136" s="1"/>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="1"/>
       <c r="B137" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C137" s="18" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
       <c r="D137" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E137" s="9"/>
       <c r="F137" s="9"/>
       <c r="G137" s="18" t="s">
-        <v>95</v>
+        <v>22</v>
       </c>
       <c r="H137" s="1"/>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="1"/>
       <c r="B138" s="9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C138" s="18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E138" s="9"/>
       <c r="F138" s="9"/>
       <c r="G138" s="18" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="H138" s="1"/>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="1"/>
       <c r="B139" s="9" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C139" s="18" t="s">
-        <v>137</v>
+        <v>97</v>
       </c>
       <c r="D139" s="11" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="E139" s="9"/>
       <c r="F139" s="9"/>
       <c r="G139" s="18" t="s">
-        <v>138</v>
+        <v>6</v>
       </c>
       <c r="H139" s="1"/>
     </row>
@@ -3170,424 +3172,424 @@
         <v>77</v>
       </c>
       <c r="C140" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D140" s="11" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
       <c r="G140" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="1"/>
       <c r="B141" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C141" s="17" t="s">
-        <v>87</v>
+        <v>78</v>
+      </c>
+      <c r="C141" s="18" t="s">
+        <v>140</v>
       </c>
       <c r="D141" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="E141" s="9"/>
-      <c r="F141" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G141" s="18" t="s">
-        <v>142</v>
-      </c>
       <c r="H141" s="1"/>
     </row>
-    <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1"/>
       <c r="B142" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C142" s="18" t="s">
-        <v>46</v>
+        <v>82</v>
+      </c>
+      <c r="C142" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="D142" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E142" s="9"/>
-      <c r="F142" s="14" t="s">
+      <c r="F142" s="9" t="s">
         <v>13</v>
       </c>
       <c r="G142" s="18" t="s">
-        <v>52</v>
+        <v>143</v>
       </c>
       <c r="H142" s="1"/>
     </row>
-    <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1"/>
       <c r="B143" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C143" s="18" t="s">
-        <v>143</v>
+        <v>46</v>
       </c>
       <c r="D143" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E143" s="9"/>
+      <c r="F143" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G143" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H143" s="1"/>
+    </row>
+    <row r="144" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="1"/>
+      <c r="B144" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C144" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="E143" s="9"/>
-      <c r="F143" s="9"/>
-      <c r="G143" s="18" t="s">
+      <c r="D144" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="H143" s="1"/>
-    </row>
-    <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="1"/>
-      <c r="B144" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="6"/>
-      <c r="F144" s="6"/>
-      <c r="G144" s="6"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="18" t="s">
+        <v>146</v>
+      </c>
       <c r="H144" s="1"/>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="1"/>
-      <c r="B145" s="7" t="s">
+      <c r="B145" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C145" s="6"/>
+      <c r="D145" s="6"/>
+      <c r="E145" s="6"/>
+      <c r="F145" s="6"/>
+      <c r="G145" s="6"/>
+      <c r="H145" s="1"/>
+    </row>
+    <row r="146" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A146" s="1"/>
+      <c r="B146" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C145" s="7" t="s">
+      <c r="C146" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D145" s="7"/>
-      <c r="E145" s="8" t="s">
+      <c r="D146" s="7"/>
+      <c r="E146" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F145" s="8" t="s">
+      <c r="F146" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G145" s="8"/>
-      <c r="H145" s="1"/>
-    </row>
-    <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1"/>
-      <c r="B146" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C146" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D146" s="10"/>
-      <c r="E146" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F146" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G146" s="11"/>
+      <c r="G146" s="8"/>
       <c r="H146" s="1"/>
     </row>
-    <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="1"/>
       <c r="B147" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C147" s="10" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="D147" s="10"/>
-      <c r="E147" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F147" s="16" t="s">
-        <v>87</v>
+      <c r="E147" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F147" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="G147" s="11"/>
       <c r="H147" s="1"/>
     </row>
-    <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="1"/>
+      <c r="B148" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D148" s="10"/>
+      <c r="E148" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F148" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G148" s="11"/>
       <c r="H148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="1"/>
-      <c r="B149" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C149" s="5"/>
-      <c r="D149" s="5"/>
-      <c r="E149" s="5"/>
-      <c r="F149" s="5"/>
-      <c r="G149" s="5"/>
       <c r="H149" s="1"/>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="1"/>
-      <c r="B150" s="6" t="s">
+      <c r="B150" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="C150" s="6"/>
-      <c r="D150" s="6"/>
-      <c r="E150" s="6"/>
-      <c r="F150" s="6"/>
-      <c r="G150" s="6"/>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5"/>
+      <c r="E150" s="5"/>
+      <c r="F150" s="5"/>
+      <c r="G150" s="5"/>
       <c r="H150" s="1"/>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
-      <c r="B151" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C151" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D151" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E151" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F151" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G151" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="B151" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
       <c r="H151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A152" s="1"/>
-      <c r="B152" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C152" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D152" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E152" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F152" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G152" s="18" t="s">
-        <v>142</v>
+      <c r="B152" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D152" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E152" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F152" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G152" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="H152" s="1"/>
     </row>
-    <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1"/>
       <c r="B153" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C153" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D153" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D153" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="E153" s="9"/>
+      <c r="E153" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="F153" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G153" s="18" t="s">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="H153" s="1"/>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="1"/>
       <c r="B154" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C154" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D154" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C154" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D154" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E154" s="19"/>
-      <c r="F154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="19" t="s">
+        <v>13</v>
+      </c>
       <c r="G154" s="18" t="s">
-        <v>149</v>
+        <v>76</v>
       </c>
       <c r="H154" s="1"/>
     </row>
-    <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1"/>
       <c r="B155" s="9" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C155" s="18" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
       <c r="D155" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="E155" s="9"/>
+        <v>12</v>
+      </c>
+      <c r="E155" s="19"/>
       <c r="F155" s="9"/>
       <c r="G155" s="18" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="H155" s="1"/>
     </row>
-    <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1"/>
       <c r="B156" s="9" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="C156" s="18" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D156" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E156" s="9"/>
       <c r="F156" s="9"/>
       <c r="G156" s="18" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="H156" s="1"/>
     </row>
-    <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1"/>
       <c r="B157" s="9" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C157" s="18" t="s">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="D157" s="11" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="E157" s="9"/>
       <c r="F157" s="9"/>
       <c r="G157" s="18" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="H157" s="1"/>
     </row>
-    <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1"/>
       <c r="B158" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C158" s="18" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="D158" s="11" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="E158" s="9"/>
       <c r="F158" s="9"/>
       <c r="G158" s="18" t="s">
-        <v>6</v>
+        <v>152</v>
       </c>
       <c r="H158" s="1"/>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="1"/>
       <c r="B159" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C159" s="18" t="s">
-        <v>152</v>
+        <v>97</v>
       </c>
       <c r="D159" s="11" t="s">
-        <v>153</v>
+        <v>98</v>
       </c>
       <c r="E159" s="9"/>
       <c r="F159" s="9"/>
       <c r="G159" s="18" t="s">
-        <v>154</v>
+        <v>6</v>
       </c>
       <c r="H159" s="1"/>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="1"/>
       <c r="B160" s="9" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="C160" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D160" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E160" s="9"/>
       <c r="F160" s="9"/>
       <c r="G160" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H160" s="1"/>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="1"/>
       <c r="B161" s="9" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C161" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D161" s="11" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="E161" s="9"/>
       <c r="F161" s="9"/>
       <c r="G161" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H161" s="1"/>
     </row>
-    <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1"/>
       <c r="B162" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C162" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D162" s="11" t="s">
-        <v>55</v>
+        <v>142</v>
       </c>
       <c r="E162" s="9"/>
       <c r="F162" s="9"/>
       <c r="G162" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H162" s="1"/>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="1"/>
       <c r="B163" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C163" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D163" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E163" s="9"/>
       <c r="F163" s="9"/>
       <c r="G163" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H163" s="1"/>
     </row>
-    <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1"/>
       <c r="B164" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C164" s="18" t="s">
-        <v>122</v>
+        <v>162</v>
       </c>
       <c r="D164" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E164" s="9"/>
       <c r="F164" s="9"/>
@@ -3596,162 +3598,162 @@
       </c>
       <c r="H164" s="1"/>
     </row>
-    <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1"/>
       <c r="B165" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C165" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D165" s="20" t="s">
-        <v>165</v>
+        <v>123</v>
+      </c>
+      <c r="D165" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="E165" s="9"/>
       <c r="F165" s="9"/>
       <c r="G165" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H165" s="1"/>
     </row>
-    <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1"/>
       <c r="B166" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C166" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D166" s="20" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="E166" s="9"/>
       <c r="F166" s="9"/>
       <c r="G166" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H166" s="1"/>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A167" s="1"/>
       <c r="B167" s="9" t="s">
-        <v>169</v>
+        <v>130</v>
       </c>
       <c r="C167" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D167" s="20" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E167" s="9"/>
       <c r="F167" s="9"/>
       <c r="G167" s="18" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H167" s="1"/>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
       <c r="B168" s="9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C168" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="D168" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E168" s="14" t="s">
-        <v>13</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D168" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E168" s="9"/>
       <c r="F168" s="9"/>
       <c r="G168" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H168" s="1"/>
     </row>
-    <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
       <c r="B169" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C169" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D169" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E169" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F169" s="9"/>
+      <c r="G169" s="18" t="s">
         <v>175</v>
       </c>
-      <c r="C169" s="18" t="s">
+      <c r="H169" s="1"/>
+    </row>
+    <row r="170" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="1"/>
+      <c r="B170" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C170" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D169" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E169" s="9"/>
-      <c r="F169" s="19" t="s">
+      <c r="D170" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="E170" s="9"/>
+      <c r="F170" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G169" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="H169" s="1"/>
-    </row>
-    <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1"/>
-      <c r="B170" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C170" s="6"/>
-      <c r="D170" s="6"/>
-      <c r="E170" s="6"/>
-      <c r="F170" s="6"/>
-      <c r="G170" s="6"/>
+      <c r="G170" s="18" t="s">
+        <v>56</v>
+      </c>
       <c r="H170" s="1"/>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
-      <c r="B171" s="7" t="s">
+      <c r="B171" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C171" s="6"/>
+      <c r="D171" s="6"/>
+      <c r="E171" s="6"/>
+      <c r="F171" s="6"/>
+      <c r="G171" s="6"/>
+      <c r="H171" s="1"/>
+    </row>
+    <row r="172" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A172" s="1"/>
+      <c r="B172" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C171" s="7" t="s">
+      <c r="C172" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D171" s="7"/>
-      <c r="E171" s="8" t="s">
+      <c r="D172" s="7"/>
+      <c r="E172" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F171" s="8" t="s">
+      <c r="F172" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G171" s="8"/>
-      <c r="H171" s="1"/>
-    </row>
-    <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1"/>
-      <c r="B172" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C172" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D172" s="10"/>
-      <c r="E172" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="F172" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="G172" s="11"/>
+      <c r="G172" s="8"/>
       <c r="H172" s="1"/>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="1"/>
       <c r="B173" s="9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C173" s="10" t="s">
-        <v>130</v>
+        <v>58</v>
       </c>
       <c r="D173" s="10"/>
-      <c r="E173" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F173" s="16" t="s">
-        <v>87</v>
+      <c r="E173" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F173" s="11" t="s">
+        <v>46</v>
       </c>
       <c r="G173" s="11"/>
       <c r="H173" s="1"/>
@@ -3762,29 +3764,46 @@
         <v>15</v>
       </c>
       <c r="C174" s="10" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="D174" s="10"/>
-      <c r="E174" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F174" s="17" t="s">
-        <v>60</v>
+      <c r="E174" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F174" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="G174" s="11"/>
       <c r="H174" s="1"/>
     </row>
-    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="21"/>
-      <c r="B175" s="1"/>
-      <c r="C175" s="1"/>
-      <c r="D175" s="1"/>
-      <c r="E175" s="1"/>
-      <c r="F175" s="1"/>
-      <c r="G175" s="1"/>
-      <c r="H175" s="21"/>
-    </row>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A175" s="1"/>
+      <c r="B175" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C175" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D175" s="10"/>
+      <c r="E175" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F175" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G175" s="11"/>
+      <c r="H175" s="1"/>
+    </row>
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="21"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="1"/>
+      <c r="E176" s="1"/>
+      <c r="F176" s="1"/>
+      <c r="G176" s="1"/>
+      <c r="H176" s="21"/>
+    </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4624,6 +4643,7 @@
     <row r="1013" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1014" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1015" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1016" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="70">
     <mergeCell ref="B2:G2"/>
@@ -4650,52 +4670,52 @@
     <mergeCell ref="B37:G37"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="B46:G46"/>
     <mergeCell ref="C47:D47"/>
-    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="C48:D48"/>
     <mergeCell ref="B50:G50"/>
-    <mergeCell ref="B57:G57"/>
-    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B58:G58"/>
     <mergeCell ref="C59:D59"/>
     <mergeCell ref="C60:D60"/>
-    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="C61:D61"/>
     <mergeCell ref="B63:G63"/>
-    <mergeCell ref="B70:G70"/>
-    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B71:G71"/>
     <mergeCell ref="C72:D72"/>
-    <mergeCell ref="B74:G74"/>
+    <mergeCell ref="C73:D73"/>
     <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="B76:G76"/>
+    <mergeCell ref="B86:G86"/>
     <mergeCell ref="C87:D87"/>
     <mergeCell ref="C88:D88"/>
-    <mergeCell ref="B90:G90"/>
+    <mergeCell ref="C89:D89"/>
     <mergeCell ref="B91:G91"/>
-    <mergeCell ref="B101:G101"/>
-    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="B92:G92"/>
+    <mergeCell ref="B102:G102"/>
     <mergeCell ref="C103:D103"/>
     <mergeCell ref="C104:D104"/>
-    <mergeCell ref="B106:G106"/>
+    <mergeCell ref="C105:D105"/>
     <mergeCell ref="B107:G107"/>
-    <mergeCell ref="B125:G125"/>
-    <mergeCell ref="C126:D126"/>
+    <mergeCell ref="B108:G108"/>
+    <mergeCell ref="B126:G126"/>
     <mergeCell ref="C127:D127"/>
     <mergeCell ref="C128:D128"/>
     <mergeCell ref="C129:D129"/>
-    <mergeCell ref="B131:G131"/>
+    <mergeCell ref="C130:D130"/>
     <mergeCell ref="B132:G132"/>
-    <mergeCell ref="B144:G144"/>
-    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="B133:G133"/>
+    <mergeCell ref="B145:G145"/>
     <mergeCell ref="C146:D146"/>
     <mergeCell ref="C147:D147"/>
-    <mergeCell ref="B149:G149"/>
+    <mergeCell ref="C148:D148"/>
     <mergeCell ref="B150:G150"/>
-    <mergeCell ref="B170:G170"/>
-    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="B151:G151"/>
+    <mergeCell ref="B171:G171"/>
     <mergeCell ref="C172:D172"/>
     <mergeCell ref="C173:D173"/>
     <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C175:D175"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4712,17 +4732,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:G13 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="7.62"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5722,10 +5757,10 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B5:G13 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="7.62"/>
   </cols>

</xml_diff>